<commit_message>
Update Tablas Lab 4 Maquina 2.xlsx
</commit_message>
<xml_diff>
--- a/Docs/Tablas Lab 4 Maquina 2.xlsx
+++ b/Docs/Tablas Lab 4 Maquina 2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -1033,11 +1033,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="193318688"/>
-        <c:axId val="193321808"/>
+        <c:axId val="193916544"/>
+        <c:axId val="193919936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="193318688"/>
+        <c:axId val="193916544"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1156,12 +1156,12 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="193321808"/>
+        <c:crossAx val="193919936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="193321808"/>
+        <c:axId val="193919936"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1280,7 +1280,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="193318688"/>
+        <c:crossAx val="193916544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1886,11 +1886,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="150572880"/>
-        <c:axId val="150576272"/>
+        <c:axId val="195103792"/>
+        <c:axId val="195107184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="150572880"/>
+        <c:axId val="195103792"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2009,12 +2009,12 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150576272"/>
+        <c:crossAx val="195107184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="150576272"/>
+        <c:axId val="195107184"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2133,7 +2133,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150572880"/>
+        <c:crossAx val="195103792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2507,7 +2507,8 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="power"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -2616,11 +2617,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="143926768"/>
-        <c:axId val="32372128"/>
+        <c:axId val="193943104"/>
+        <c:axId val="193946496"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="143926768"/>
+        <c:axId val="193943104"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2739,12 +2740,12 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="32372128"/>
+        <c:crossAx val="193946496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="32372128"/>
+        <c:axId val="193946496"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -2858,7 +2859,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="143926768"/>
+        <c:crossAx val="193943104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3337,11 +3338,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="150254400"/>
-        <c:axId val="150257792"/>
+        <c:axId val="195146016"/>
+        <c:axId val="195149776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="150254400"/>
+        <c:axId val="195146016"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3460,12 +3461,12 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150257792"/>
+        <c:crossAx val="195149776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="150257792"/>
+        <c:axId val="195149776"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -3579,7 +3580,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="150254400"/>
+        <c:crossAx val="195146016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4069,11 +4070,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="67903440"/>
-        <c:axId val="122188416"/>
+        <c:axId val="195196864"/>
+        <c:axId val="195200624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="67903440"/>
+        <c:axId val="195196864"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4192,12 +4193,12 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122188416"/>
+        <c:crossAx val="195200624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="122188416"/>
+        <c:axId val="195200624"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -4311,7 +4312,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="67903440"/>
+        <c:crossAx val="195196864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7172,7 +7173,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="106" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="106" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7216,7 +7217,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="118" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7233,7 +7234,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F86A8C9-B823-4237-B971-35F9FC141626}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1F86A8C9-B823-4237-B971-35F9FC141626}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7266,7 +7267,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F79FD9B3-1053-4105-BF53-EDCA2C102566}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F79FD9B3-1053-4105-BF53-EDCA2C102566}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7299,7 +7300,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E62ACB43-BF23-44E0-A2C1-1BE0D48E226C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E62ACB43-BF23-44E0-A2C1-1BE0D48E226C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7332,7 +7333,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CD62A27-62EF-4A76-950F-A06EC21FDB46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{6CD62A27-62EF-4A76-950F-A06EC21FDB46}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7359,13 +7360,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8663983" cy="6285424"/>
+    <xdr:ext cx="8674919" cy="6288548"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49C9A0CC-8523-4ADB-8134-5F68720F3C67}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{49C9A0CC-8523-4ADB-8134-5F68720F3C67}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>